<commit_message>
Cleaning, adjusting to new spreadsheet
</commit_message>
<xml_diff>
--- a/Example/Filled/2023_09_31___BSP_AR1_ST.w.8.7.5.xlsx
+++ b/Example/Filled/2023_09_31___BSP_AR1_ST.w.8.7.5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzysztof kaniewski\PycharmProjects\pythonProject\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzysztof kaniewski\PycharmProjects\pythonProject\Example\Filled\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CEDB33-E7E6-426D-A74E-F3A40401A651}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1921D568-C0CF-4EFE-9D25-5F93D37B780B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="830" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEO6" sheetId="18" r:id="rId1"/>
@@ -5409,10 +5409,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5424,34 +5445,13 @@
     <xf numFmtId="0" fontId="32" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9352,8 +9352,8 @@
   </sheetPr>
   <dimension ref="A2:P30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10474,7 +10474,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11311,7 +11311,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12291,8 +12291,8 @@
   </sheetPr>
   <dimension ref="A1:AY968"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26553,18 +26553,18 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="220" t="s">
+      <c r="N3" s="232" t="s">
         <v>111</v>
       </c>
-      <c r="O3" s="220"/>
-      <c r="P3" s="220"/>
-      <c r="Q3" s="220"/>
-      <c r="R3" s="220" t="s">
+      <c r="O3" s="232"/>
+      <c r="P3" s="232"/>
+      <c r="Q3" s="232"/>
+      <c r="R3" s="232" t="s">
         <v>112</v>
       </c>
-      <c r="S3" s="220"/>
-      <c r="T3" s="220"/>
-      <c r="U3" s="220"/>
+      <c r="S3" s="232"/>
+      <c r="T3" s="232"/>
+      <c r="U3" s="232"/>
       <c r="V3" s="183"/>
       <c r="W3" s="183"/>
       <c r="X3" s="183"/>
@@ -26590,22 +26590,22 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="220" t="s">
+      <c r="N4" s="232" t="s">
         <v>835</v>
       </c>
-      <c r="O4" s="220"/>
-      <c r="P4" s="220" t="s">
+      <c r="O4" s="232"/>
+      <c r="P4" s="232" t="s">
         <v>980</v>
       </c>
-      <c r="Q4" s="220"/>
-      <c r="R4" s="220" t="s">
+      <c r="Q4" s="232"/>
+      <c r="R4" s="232" t="s">
         <v>981</v>
       </c>
-      <c r="S4" s="220"/>
-      <c r="T4" s="220" t="s">
+      <c r="S4" s="232"/>
+      <c r="T4" s="232" t="s">
         <v>982</v>
       </c>
-      <c r="U4" s="220"/>
+      <c r="U4" s="232"/>
       <c r="V4" s="183"/>
       <c r="W4" s="183"/>
       <c r="X4" s="183"/>
@@ -26729,18 +26729,18 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="221" t="s">
+      <c r="N7" s="222" t="s">
         <v>205</v>
       </c>
-      <c r="O7" s="221"/>
-      <c r="P7" s="221"/>
-      <c r="Q7" s="221"/>
-      <c r="R7" s="221" t="s">
+      <c r="O7" s="222"/>
+      <c r="P7" s="222"/>
+      <c r="Q7" s="222"/>
+      <c r="R7" s="222" t="s">
         <v>249</v>
       </c>
-      <c r="S7" s="221"/>
-      <c r="T7" s="221"/>
-      <c r="U7" s="221"/>
+      <c r="S7" s="222"/>
+      <c r="T7" s="222"/>
+      <c r="U7" s="222"/>
       <c r="V7" s="183"/>
       <c r="W7" s="183"/>
       <c r="X7" s="183"/>
@@ -26766,22 +26766,22 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="231" t="s">
+      <c r="N8" s="233" t="s">
         <v>201</v>
       </c>
-      <c r="O8" s="232"/>
-      <c r="P8" s="231" t="s">
+      <c r="O8" s="234"/>
+      <c r="P8" s="233" t="s">
         <v>202</v>
       </c>
-      <c r="Q8" s="232"/>
-      <c r="R8" s="221" t="s">
+      <c r="Q8" s="234"/>
+      <c r="R8" s="222" t="s">
         <v>253</v>
       </c>
-      <c r="S8" s="221"/>
-      <c r="T8" s="221" t="s">
+      <c r="S8" s="222"/>
+      <c r="T8" s="222" t="s">
         <v>252</v>
       </c>
-      <c r="U8" s="221"/>
+      <c r="U8" s="222"/>
       <c r="V8" s="183"/>
       <c r="W8" s="183"/>
       <c r="X8" s="183"/>
@@ -26852,25 +26852,25 @@
       <c r="E10" s="91" t="s">
         <v>148</v>
       </c>
-      <c r="F10" s="234" t="s">
+      <c r="F10" s="220" t="s">
         <v>254</v>
       </c>
-      <c r="G10" s="233" t="s">
+      <c r="G10" s="221" t="s">
         <v>87</v>
       </c>
-      <c r="H10" s="233" t="s">
+      <c r="H10" s="221" t="s">
         <v>16</v>
       </c>
       <c r="I10" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="221" t="s">
+      <c r="J10" s="222" t="s">
         <v>833</v>
       </c>
-      <c r="K10" s="222" t="s">
+      <c r="K10" s="229" t="s">
         <v>206</v>
       </c>
-      <c r="L10" s="221" t="s">
+      <c r="L10" s="222" t="s">
         <v>208</v>
       </c>
       <c r="M10" s="82" t="s">
@@ -26925,15 +26925,15 @@
       <c r="E11" s="91" t="s">
         <v>162</v>
       </c>
-      <c r="F11" s="234"/>
-      <c r="G11" s="233"/>
-      <c r="H11" s="233"/>
+      <c r="F11" s="220"/>
+      <c r="G11" s="221"/>
+      <c r="H11" s="221"/>
       <c r="I11" s="73" t="s">
         <v>972</v>
       </c>
-      <c r="J11" s="221"/>
-      <c r="K11" s="223"/>
-      <c r="L11" s="221"/>
+      <c r="J11" s="222"/>
+      <c r="K11" s="230"/>
+      <c r="L11" s="222"/>
       <c r="M11" s="82" t="s">
         <v>973</v>
       </c>
@@ -26986,15 +26986,15 @@
       <c r="E12" s="91" t="s">
         <v>149</v>
       </c>
-      <c r="F12" s="234"/>
-      <c r="G12" s="233"/>
-      <c r="H12" s="233"/>
+      <c r="F12" s="220"/>
+      <c r="G12" s="221"/>
+      <c r="H12" s="221"/>
       <c r="I12" s="122" t="s">
         <v>209</v>
       </c>
-      <c r="J12" s="221"/>
-      <c r="K12" s="223"/>
-      <c r="L12" s="221"/>
+      <c r="J12" s="222"/>
+      <c r="K12" s="230"/>
+      <c r="L12" s="222"/>
       <c r="M12" s="123" t="s">
         <v>209</v>
       </c>
@@ -27047,15 +27047,15 @@
       <c r="E13" s="91" t="s">
         <v>150</v>
       </c>
-      <c r="F13" s="234"/>
-      <c r="G13" s="233"/>
-      <c r="H13" s="233"/>
+      <c r="F13" s="220"/>
+      <c r="G13" s="221"/>
+      <c r="H13" s="221"/>
       <c r="I13" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="221"/>
-      <c r="K13" s="223"/>
-      <c r="L13" s="221"/>
+      <c r="J13" s="222"/>
+      <c r="K13" s="230"/>
+      <c r="L13" s="222"/>
       <c r="M13" s="123" t="s">
         <v>53</v>
       </c>
@@ -27104,17 +27104,17 @@
       <c r="E14" s="91" t="s">
         <v>151</v>
       </c>
-      <c r="F14" s="234"/>
-      <c r="G14" s="233"/>
-      <c r="H14" s="233" t="s">
+      <c r="F14" s="220"/>
+      <c r="G14" s="221"/>
+      <c r="H14" s="221" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="221"/>
-      <c r="K14" s="223"/>
-      <c r="L14" s="221" t="s">
+      <c r="J14" s="222"/>
+      <c r="K14" s="230"/>
+      <c r="L14" s="222" t="s">
         <v>207</v>
       </c>
       <c r="M14" s="82" t="s">
@@ -27169,15 +27169,15 @@
       <c r="E15" s="91" t="s">
         <v>163</v>
       </c>
-      <c r="F15" s="234"/>
-      <c r="G15" s="233"/>
-      <c r="H15" s="233"/>
+      <c r="F15" s="220"/>
+      <c r="G15" s="221"/>
+      <c r="H15" s="221"/>
       <c r="I15" s="73" t="s">
         <v>972</v>
       </c>
-      <c r="J15" s="221"/>
-      <c r="K15" s="223"/>
-      <c r="L15" s="221"/>
+      <c r="J15" s="222"/>
+      <c r="K15" s="230"/>
+      <c r="L15" s="222"/>
       <c r="M15" s="82" t="s">
         <v>969</v>
       </c>
@@ -27230,15 +27230,15 @@
       <c r="E16" s="91" t="s">
         <v>152</v>
       </c>
-      <c r="F16" s="234"/>
-      <c r="G16" s="233"/>
-      <c r="H16" s="233"/>
+      <c r="F16" s="220"/>
+      <c r="G16" s="221"/>
+      <c r="H16" s="221"/>
       <c r="I16" s="74" t="s">
         <v>209</v>
       </c>
-      <c r="J16" s="221"/>
-      <c r="K16" s="223"/>
-      <c r="L16" s="221"/>
+      <c r="J16" s="222"/>
+      <c r="K16" s="230"/>
+      <c r="L16" s="222"/>
       <c r="M16" s="123" t="s">
         <v>209</v>
       </c>
@@ -27291,15 +27291,15 @@
       <c r="E17" s="91" t="s">
         <v>153</v>
       </c>
-      <c r="F17" s="234"/>
-      <c r="G17" s="233"/>
-      <c r="H17" s="233"/>
+      <c r="F17" s="220"/>
+      <c r="G17" s="221"/>
+      <c r="H17" s="221"/>
       <c r="I17" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="J17" s="221"/>
-      <c r="K17" s="224"/>
-      <c r="L17" s="221"/>
+      <c r="J17" s="222"/>
+      <c r="K17" s="231"/>
+      <c r="L17" s="222"/>
       <c r="M17" s="123" t="s">
         <v>53</v>
       </c>
@@ -27348,19 +27348,19 @@
       <c r="E18" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="234"/>
-      <c r="G18" s="233" t="s">
+      <c r="F18" s="220"/>
+      <c r="G18" s="221" t="s">
         <v>88</v>
       </c>
-      <c r="H18" s="233"/>
+      <c r="H18" s="221"/>
       <c r="I18" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="J18" s="221"/>
-      <c r="K18" s="225" t="s">
+      <c r="J18" s="222"/>
+      <c r="K18" s="223" t="s">
         <v>974</v>
       </c>
-      <c r="L18" s="226"/>
+      <c r="L18" s="224"/>
       <c r="M18" s="123" t="s">
         <v>53</v>
       </c>
@@ -27413,13 +27413,13 @@
       <c r="E19" s="90" t="s">
         <v>977</v>
       </c>
-      <c r="F19" s="234"/>
-      <c r="G19" s="233"/>
-      <c r="H19" s="233"/>
+      <c r="F19" s="220"/>
+      <c r="G19" s="221"/>
+      <c r="H19" s="221"/>
       <c r="I19" s="73" t="s">
         <v>978</v>
       </c>
-      <c r="J19" s="221"/>
+      <c r="J19" s="222"/>
       <c r="K19" s="227"/>
       <c r="L19" s="228"/>
       <c r="M19" s="71" t="s">
@@ -27470,19 +27470,19 @@
       <c r="E20" s="91" t="s">
         <v>146</v>
       </c>
-      <c r="F20" s="234"/>
-      <c r="G20" s="233" t="s">
+      <c r="F20" s="220"/>
+      <c r="G20" s="221" t="s">
         <v>89</v>
       </c>
-      <c r="H20" s="233"/>
+      <c r="H20" s="221"/>
       <c r="I20" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="J20" s="221"/>
-      <c r="K20" s="225" t="s">
+      <c r="J20" s="222"/>
+      <c r="K20" s="223" t="s">
         <v>975</v>
       </c>
-      <c r="L20" s="226"/>
+      <c r="L20" s="224"/>
       <c r="M20" s="82" t="s">
         <v>183</v>
       </c>
@@ -27535,15 +27535,15 @@
       <c r="E21" s="91" t="s">
         <v>147</v>
       </c>
-      <c r="F21" s="234"/>
-      <c r="G21" s="233"/>
-      <c r="H21" s="233"/>
+      <c r="F21" s="220"/>
+      <c r="G21" s="221"/>
+      <c r="H21" s="221"/>
       <c r="I21" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="221"/>
-      <c r="K21" s="229"/>
-      <c r="L21" s="230"/>
+      <c r="J21" s="222"/>
+      <c r="K21" s="225"/>
+      <c r="L21" s="226"/>
       <c r="M21" s="123" t="s">
         <v>53</v>
       </c>
@@ -27596,13 +27596,13 @@
       <c r="E22" s="91" t="s">
         <v>177</v>
       </c>
-      <c r="F22" s="234"/>
-      <c r="G22" s="233"/>
-      <c r="H22" s="233"/>
+      <c r="F22" s="220"/>
+      <c r="G22" s="221"/>
+      <c r="H22" s="221"/>
       <c r="I22" s="73" t="s">
         <v>971</v>
       </c>
-      <c r="J22" s="221"/>
+      <c r="J22" s="222"/>
       <c r="K22" s="227"/>
       <c r="L22" s="228"/>
       <c r="M22" s="71" t="s">
@@ -27657,19 +27657,19 @@
       <c r="E23" s="90" t="s">
         <v>154</v>
       </c>
-      <c r="F23" s="234"/>
-      <c r="G23" s="233" t="s">
+      <c r="F23" s="220"/>
+      <c r="G23" s="221" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="233"/>
+      <c r="H23" s="221"/>
       <c r="I23" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="J23" s="221"/>
-      <c r="K23" s="225" t="s">
+      <c r="J23" s="222"/>
+      <c r="K23" s="223" t="s">
         <v>976</v>
       </c>
-      <c r="L23" s="226"/>
+      <c r="L23" s="224"/>
       <c r="M23" s="71" t="s">
         <v>183</v>
       </c>
@@ -27722,15 +27722,15 @@
       <c r="E24" s="90" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="234"/>
-      <c r="G24" s="233"/>
-      <c r="H24" s="233"/>
+      <c r="F24" s="220"/>
+      <c r="G24" s="221"/>
+      <c r="H24" s="221"/>
       <c r="I24" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="221"/>
-      <c r="K24" s="229"/>
-      <c r="L24" s="230"/>
+      <c r="J24" s="222"/>
+      <c r="K24" s="225"/>
+      <c r="L24" s="226"/>
       <c r="M24" s="123" t="s">
         <v>53</v>
       </c>
@@ -27783,13 +27783,13 @@
       <c r="E25" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="F25" s="234"/>
-      <c r="G25" s="233"/>
-      <c r="H25" s="233"/>
+      <c r="F25" s="220"/>
+      <c r="G25" s="221"/>
+      <c r="H25" s="221"/>
       <c r="I25" s="73" t="s">
         <v>971</v>
       </c>
-      <c r="J25" s="221"/>
+      <c r="J25" s="222"/>
       <c r="K25" s="227"/>
       <c r="L25" s="228"/>
       <c r="M25" s="71" t="s">
@@ -27844,25 +27844,25 @@
       <c r="E26" s="91" t="s">
         <v>156</v>
       </c>
-      <c r="F26" s="234" t="s">
+      <c r="F26" s="220" t="s">
         <v>970</v>
       </c>
-      <c r="G26" s="233" t="s">
+      <c r="G26" s="221" t="s">
         <v>87</v>
       </c>
-      <c r="H26" s="233" t="s">
+      <c r="H26" s="221" t="s">
         <v>16</v>
       </c>
       <c r="I26" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="J26" s="221" t="s">
+      <c r="J26" s="222" t="s">
         <v>836</v>
       </c>
-      <c r="K26" s="222" t="s">
+      <c r="K26" s="229" t="s">
         <v>206</v>
       </c>
-      <c r="L26" s="221" t="s">
+      <c r="L26" s="222" t="s">
         <v>208</v>
       </c>
       <c r="M26" s="82" t="s">
@@ -27913,15 +27913,15 @@
       <c r="E27" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="F27" s="234"/>
-      <c r="G27" s="233"/>
-      <c r="H27" s="233"/>
+      <c r="F27" s="220"/>
+      <c r="G27" s="221"/>
+      <c r="H27" s="221"/>
       <c r="I27" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="J27" s="221"/>
-      <c r="K27" s="223"/>
-      <c r="L27" s="221"/>
+      <c r="J27" s="222"/>
+      <c r="K27" s="230"/>
+      <c r="L27" s="222"/>
       <c r="M27" s="123" t="s">
         <v>53</v>
       </c>
@@ -27970,17 +27970,17 @@
       <c r="E28" s="91" t="s">
         <v>158</v>
       </c>
-      <c r="F28" s="234"/>
-      <c r="G28" s="233"/>
-      <c r="H28" s="233" t="s">
+      <c r="F28" s="220"/>
+      <c r="G28" s="221"/>
+      <c r="H28" s="221" t="s">
         <v>17</v>
       </c>
       <c r="I28" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="J28" s="221"/>
-      <c r="K28" s="223"/>
-      <c r="L28" s="221" t="s">
+      <c r="J28" s="222"/>
+      <c r="K28" s="230"/>
+      <c r="L28" s="222" t="s">
         <v>207</v>
       </c>
       <c r="M28" s="71" t="s">
@@ -28031,15 +28031,15 @@
       <c r="E29" s="91" t="s">
         <v>159</v>
       </c>
-      <c r="F29" s="234"/>
-      <c r="G29" s="233"/>
-      <c r="H29" s="233"/>
+      <c r="F29" s="220"/>
+      <c r="G29" s="221"/>
+      <c r="H29" s="221"/>
       <c r="I29" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="J29" s="221"/>
-      <c r="K29" s="224"/>
-      <c r="L29" s="221"/>
+      <c r="J29" s="222"/>
+      <c r="K29" s="231"/>
+      <c r="L29" s="222"/>
       <c r="M29" s="72" t="s">
         <v>53</v>
       </c>
@@ -28244,6 +28244,25 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J10:J25"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="K10:K17"/>
+    <mergeCell ref="K18:L19"/>
+    <mergeCell ref="K20:L22"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="G20:H22"/>
     <mergeCell ref="F26:F29"/>
     <mergeCell ref="G26:G29"/>
     <mergeCell ref="J26:J29"/>
@@ -28258,26 +28277,7 @@
     <mergeCell ref="G18:H19"/>
     <mergeCell ref="H26:H27"/>
     <mergeCell ref="H28:H29"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="G20:H22"/>
     <mergeCell ref="G23:H25"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="J10:J25"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="K10:K17"/>
-    <mergeCell ref="K18:L19"/>
-    <mergeCell ref="K20:L22"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="P4:Q4"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>